<commit_message>
RDM-5690 - fixed issue with last auto merge.
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sateesh/moj/workspace/ccd/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0F90A6-9359-1C41-A65F-BFA334F61047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8482A7DC-2EA5-A947-8A69-2438D283D875}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="16640" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="363">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1159,6 +1159,12 @@
   </si>
   <si>
     <t>Test Description</t>
+  </si>
+  <si>
+    <t>[LAST_STATE_MODIFIED_DATE]</t>
+  </si>
+  <si>
+    <t>Last State Modified Date</t>
   </si>
 </sst>
 </file>
@@ -1757,7 +1763,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2028,6 +2034,9 @@
     <xf numFmtId="49" fontId="43" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="44" fillId="2" borderId="1" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -3033,10 +3042,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3167,24 +3176,22 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="54">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="172" t="s">
-        <v>249</v>
-      </c>
-      <c r="G7" s="47">
-        <v>2</v>
+      <c r="A7" s="202">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="203"/>
+      <c r="C7" s="178" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="178" t="s">
+        <v>361</v>
+      </c>
+      <c r="E7" s="204" t="s">
+        <v>362</v>
+      </c>
+      <c r="F7" s="204"/>
+      <c r="G7" s="203">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3196,14 +3203,16 @@
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>218</v>
-      </c>
-      <c r="F8" s="172"/>
+        <v>72</v>
+      </c>
+      <c r="F8" s="172" t="s">
+        <v>249</v>
+      </c>
       <c r="G8" s="47">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3215,13 +3224,32 @@
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>53</v>
+        <v>218</v>
       </c>
       <c r="F9" s="172"/>
       <c r="G9" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="54">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="47"/>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="172"/>
+      <c r="G10" s="47">
         <v>1</v>
       </c>
     </row>
@@ -8696,7 +8724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A1F88E-5CB0-9F47-9415-593D73C5FD9E}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -8727,7 +8755,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
RDM-7627 fixed failing tests
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0F90A6-9359-1C41-A65F-BFA334F61047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711B6CB4-90C1-CA43-B7B7-E86E7A053141}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="361">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3777,8 +3777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8696,7 +8696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A1F88E-5CB0-9F47-9415-593D73C5FD9E}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -8727,7 +8727,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
@@ -14410,8 +14410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18326,8 +18326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18953,9 +18953,7 @@
       <c r="K15" s="99" t="s">
         <v>267</v>
       </c>
-      <c r="L15" s="155" t="s">
-        <v>319</v>
-      </c>
+      <c r="L15" s="155"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>

</xml_diff>

<commit_message>
Revert "Upgrade to befta fw 1.1.1"
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sateesh/moj/workspace/ccd/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8482A7DC-2EA5-A947-8A69-2438D283D875}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0F90A6-9359-1C41-A65F-BFA334F61047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="16640" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="361">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1159,12 +1159,6 @@
   </si>
   <si>
     <t>Test Description</t>
-  </si>
-  <si>
-    <t>[LAST_STATE_MODIFIED_DATE]</t>
-  </si>
-  <si>
-    <t>Last State Modified Date</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1757,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="205">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2034,9 +2028,6 @@
     <xf numFmtId="49" fontId="43" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="44" fillId="2" borderId="1" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -3042,10 +3033,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3176,22 +3167,24 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="202">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="203"/>
-      <c r="C7" s="178" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="178" t="s">
-        <v>361</v>
-      </c>
-      <c r="E7" s="204" t="s">
-        <v>362</v>
-      </c>
-      <c r="F7" s="204"/>
-      <c r="G7" s="203">
-        <v>4</v>
+      <c r="A7" s="54">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="47"/>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="172" t="s">
+        <v>249</v>
+      </c>
+      <c r="G7" s="47">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3203,16 +3196,14 @@
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="172" t="s">
-        <v>249</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="F8" s="172"/>
       <c r="G8" s="47">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3224,32 +3215,13 @@
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>218</v>
+        <v>53</v>
       </c>
       <c r="F9" s="172"/>
       <c r="G9" s="47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="54">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="172"/>
-      <c r="G10" s="47">
         <v>1</v>
       </c>
     </row>
@@ -8724,7 +8696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A1F88E-5CB0-9F47-9415-593D73C5FD9E}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -8755,7 +8727,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
undo revert on develop
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sateesh/moj/workspace/ccd/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0F90A6-9359-1C41-A65F-BFA334F61047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8482A7DC-2EA5-A947-8A69-2438D283D875}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="16640" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="363">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1159,6 +1159,12 @@
   </si>
   <si>
     <t>Test Description</t>
+  </si>
+  <si>
+    <t>[LAST_STATE_MODIFIED_DATE]</t>
+  </si>
+  <si>
+    <t>Last State Modified Date</t>
   </si>
 </sst>
 </file>
@@ -1757,7 +1763,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2028,6 +2034,9 @@
     <xf numFmtId="49" fontId="43" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="44" fillId="2" borderId="1" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -3033,10 +3042,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3167,24 +3176,22 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="54">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="172" t="s">
-        <v>249</v>
-      </c>
-      <c r="G7" s="47">
-        <v>2</v>
+      <c r="A7" s="202">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="203"/>
+      <c r="C7" s="178" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="178" t="s">
+        <v>361</v>
+      </c>
+      <c r="E7" s="204" t="s">
+        <v>362</v>
+      </c>
+      <c r="F7" s="204"/>
+      <c r="G7" s="203">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3196,14 +3203,16 @@
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>218</v>
-      </c>
-      <c r="F8" s="172"/>
+        <v>72</v>
+      </c>
+      <c r="F8" s="172" t="s">
+        <v>249</v>
+      </c>
       <c r="G8" s="47">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3215,13 +3224,32 @@
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>53</v>
+        <v>218</v>
       </c>
       <c r="F9" s="172"/>
       <c r="G9" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="54">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="47"/>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="172"/>
+      <c r="G10" s="47">
         <v>1</v>
       </c>
     </row>
@@ -8696,7 +8724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A1F88E-5CB0-9F47-9415-593D73C5FD9E}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -8727,7 +8755,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
RDM-7627 merged dev into branch and applied my changes on top
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sateesh/moj/workspace/ccd/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8482A7DC-2EA5-A947-8A69-2438D283D875}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D3AD0C-DEB6-7945-9ED7-C2AA08BB77F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="16640" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="16640" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="363">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3044,7 +3044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -18354,8 +18354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18981,9 +18981,7 @@
       <c r="K15" s="99" t="s">
         <v>267</v>
       </c>
-      <c r="L15" s="155" t="s">
-        <v>319</v>
-      </c>
+      <c r="L15" s="155"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>

</xml_diff>

<commit_message>
RDM-7800 - updated test definition file to include showCondition on searchinput/workbasketinput tabs
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sateesh/moj/workspace/ccd/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8482A7DC-2EA5-A947-8A69-2438D283D875}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BE840D-CF1B-3E43-AE22-E55F43201CCA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="16640" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="16640" tabRatio="500" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="366">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1165,6 +1165,15 @@
   </si>
   <si>
     <t>Last State Modified Date</t>
+  </si>
+  <si>
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;</t>
+  </si>
+  <si>
+    <t>Age="30"</t>
+  </si>
+  <si>
+    <t>ContectNumber="07777777777"</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1772,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="205">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2037,6 +2046,9 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -2706,10 +2718,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F1" sqref="F1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2718,12 +2730,12 @@
     <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="20.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="1" customWidth="1"/>
-    <col min="8" max="1026" width="8.83203125" customWidth="1"/>
+    <col min="5" max="7" width="20.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" customWidth="1"/>
+    <col min="9" max="1027" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>213</v>
       </c>
@@ -2738,9 +2750,10 @@
       </c>
       <c r="E1" s="47"/>
       <c r="F1" s="177"/>
-      <c r="G1" s="47"/>
-    </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="G1" s="177"/>
+      <c r="H1" s="47"/>
+    </row>
+    <row r="2" spans="1:8" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="48"/>
       <c r="B2" s="48"/>
       <c r="C2" s="49" t="s">
@@ -2752,14 +2765,17 @@
       <c r="E2" s="49" t="s">
         <v>215</v>
       </c>
-      <c r="F2" s="165" t="s">
+      <c r="F2" s="205" t="s">
+        <v>363</v>
+      </c>
+      <c r="G2" s="165" t="s">
         <v>332</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="H2" s="49" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="50" t="s">
         <v>7</v>
       </c>
@@ -2775,14 +2791,17 @@
       <c r="E3" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="124" t="s">
+      <c r="F3" s="161" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="124" t="s">
         <v>247</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="H3" s="50" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="52">
         <v>42736</v>
       </c>
@@ -2797,11 +2816,12 @@
         <v>46</v>
       </c>
       <c r="F4" s="172"/>
-      <c r="G4" s="47">
+      <c r="G4" s="172"/>
+      <c r="H4" s="47">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52">
         <v>42736</v>
       </c>
@@ -2816,11 +2836,12 @@
         <v>53</v>
       </c>
       <c r="F5" s="172"/>
-      <c r="G5" s="47">
+      <c r="G5" s="172"/>
+      <c r="H5" s="47">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="52">
         <v>42736</v>
       </c>
@@ -2835,11 +2856,12 @@
         <v>55</v>
       </c>
       <c r="F6" s="172"/>
-      <c r="G6" s="47">
+      <c r="G6" s="172"/>
+      <c r="H6" s="47">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
         <v>42736</v>
       </c>
@@ -2853,14 +2875,15 @@
       <c r="E7" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="172" t="s">
+      <c r="F7" s="172"/>
+      <c r="G7" s="172" t="s">
         <v>249</v>
       </c>
-      <c r="G7" s="47">
+      <c r="H7" s="47">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52">
         <v>42736</v>
       </c>
@@ -2875,11 +2898,12 @@
         <v>53</v>
       </c>
       <c r="F8" s="172"/>
-      <c r="G8" s="47">
+      <c r="G8" s="172"/>
+      <c r="H8" s="47">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52">
         <v>42736</v>
       </c>
@@ -2894,11 +2918,12 @@
         <v>55</v>
       </c>
       <c r="F9" s="172"/>
-      <c r="G9" s="47">
+      <c r="G9" s="172"/>
+      <c r="H9" s="47">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52">
         <v>42736</v>
       </c>
@@ -2913,11 +2938,12 @@
         <v>72</v>
       </c>
       <c r="F10" s="172"/>
-      <c r="G10" s="47">
+      <c r="G10" s="172"/>
+      <c r="H10" s="47">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52">
         <v>42736</v>
       </c>
@@ -2932,11 +2958,12 @@
         <v>75</v>
       </c>
       <c r="F11" s="172"/>
-      <c r="G11" s="47">
+      <c r="G11" s="172"/>
+      <c r="H11" s="47">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52">
         <v>42736</v>
       </c>
@@ -2951,11 +2978,12 @@
         <v>77</v>
       </c>
       <c r="F12" s="172"/>
-      <c r="G12" s="47">
+      <c r="G12" s="172"/>
+      <c r="H12" s="47">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52">
         <v>42736</v>
       </c>
@@ -2970,11 +2998,12 @@
         <v>79</v>
       </c>
       <c r="F13" s="172"/>
-      <c r="G13" s="47">
+      <c r="G13" s="172"/>
+      <c r="H13" s="47">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52">
         <v>42736</v>
       </c>
@@ -2989,11 +3018,12 @@
         <v>82</v>
       </c>
       <c r="F14" s="172"/>
-      <c r="G14" s="47">
+      <c r="G14" s="172"/>
+      <c r="H14" s="47">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52">
         <v>42736</v>
       </c>
@@ -3008,11 +3038,12 @@
         <v>84</v>
       </c>
       <c r="F15" s="172"/>
-      <c r="G15" s="47">
+      <c r="G15" s="172"/>
+      <c r="H15" s="47">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52">
         <v>42736</v>
       </c>
@@ -3026,8 +3057,11 @@
       <c r="E16" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="172"/>
-      <c r="G16" s="47">
+      <c r="F16" s="172" t="s">
+        <v>364</v>
+      </c>
+      <c r="G16" s="172"/>
+      <c r="H16" s="47">
         <v>10</v>
       </c>
     </row>
@@ -3044,7 +3078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -3264,10 +3298,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3276,12 +3310,12 @@
     <col min="2" max="2" width="15.33203125" style="55" customWidth="1"/>
     <col min="3" max="3" width="29.83203125" style="55" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" style="55" customWidth="1"/>
-    <col min="5" max="6" width="20.1640625" style="55" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="55" customWidth="1"/>
-    <col min="8" max="1026" width="8.83203125" customWidth="1"/>
+    <col min="5" max="7" width="20.1640625" style="55" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="55" customWidth="1"/>
+    <col min="9" max="1027" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>219</v>
       </c>
@@ -3295,10 +3329,11 @@
         <v>3</v>
       </c>
       <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="F1" s="177"/>
       <c r="G1" s="60"/>
-    </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="H1" s="60"/>
+    </row>
+    <row r="2" spans="1:8" ht="80" x14ac:dyDescent="0.15">
       <c r="A2" s="61"/>
       <c r="B2" s="61"/>
       <c r="C2" s="62" t="s">
@@ -3310,14 +3345,17 @@
       <c r="E2" s="62" t="s">
         <v>222</v>
       </c>
-      <c r="F2" s="165" t="s">
+      <c r="F2" s="205" t="s">
+        <v>363</v>
+      </c>
+      <c r="G2" s="165" t="s">
         <v>332</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="H2" s="62" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="63" t="s">
         <v>7</v>
       </c>
@@ -3333,14 +3371,17 @@
       <c r="E3" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="124" t="s">
+      <c r="F3" s="161" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="124" t="s">
         <v>247</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="H3" s="63" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="52">
         <v>42736</v>
       </c>
@@ -3355,11 +3396,12 @@
         <v>46</v>
       </c>
       <c r="F4" s="172"/>
-      <c r="G4" s="47">
+      <c r="G4" s="172"/>
+      <c r="H4" s="47">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52">
         <v>42736</v>
       </c>
@@ -3373,12 +3415,13 @@
       <c r="E5" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="172"/>
-      <c r="G5" s="47">
+      <c r="F5" s="53"/>
+      <c r="G5" s="172"/>
+      <c r="H5" s="47">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="52">
         <v>42736</v>
       </c>
@@ -3393,11 +3436,12 @@
         <v>55</v>
       </c>
       <c r="F6" s="172"/>
-      <c r="G6" s="47">
+      <c r="G6" s="172"/>
+      <c r="H6" s="47">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
         <v>42736</v>
       </c>
@@ -3411,14 +3455,15 @@
       <c r="E7" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="172" t="s">
+      <c r="F7" s="172"/>
+      <c r="G7" s="172" t="s">
         <v>249</v>
       </c>
-      <c r="G7" s="47">
+      <c r="H7" s="47">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52">
         <v>42736</v>
       </c>
@@ -3433,11 +3478,12 @@
         <v>53</v>
       </c>
       <c r="F8" s="172"/>
-      <c r="G8" s="47">
+      <c r="G8" s="172"/>
+      <c r="H8" s="47">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52">
         <v>42736</v>
       </c>
@@ -3452,11 +3498,12 @@
         <v>55</v>
       </c>
       <c r="F9" s="172"/>
-      <c r="G9" s="47">
+      <c r="G9" s="172"/>
+      <c r="H9" s="47">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52">
         <v>42736</v>
       </c>
@@ -3471,11 +3518,12 @@
         <v>72</v>
       </c>
       <c r="F10" s="172"/>
-      <c r="G10" s="47">
+      <c r="G10" s="172"/>
+      <c r="H10" s="47">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52">
         <v>42736</v>
       </c>
@@ -3490,11 +3538,12 @@
         <v>75</v>
       </c>
       <c r="F11" s="172"/>
-      <c r="G11" s="47">
+      <c r="G11" s="172"/>
+      <c r="H11" s="47">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52">
         <v>42736</v>
       </c>
@@ -3509,11 +3558,12 @@
         <v>77</v>
       </c>
       <c r="F12" s="172"/>
-      <c r="G12" s="47">
+      <c r="G12" s="172"/>
+      <c r="H12" s="47">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52">
         <v>42736</v>
       </c>
@@ -3528,11 +3578,12 @@
         <v>79</v>
       </c>
       <c r="F13" s="172"/>
-      <c r="G13" s="47">
+      <c r="G13" s="172"/>
+      <c r="H13" s="47">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52">
         <v>42736</v>
       </c>
@@ -3546,12 +3597,15 @@
       <c r="E14" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="172"/>
-      <c r="G14" s="47">
+      <c r="F14" s="53" t="s">
+        <v>365</v>
+      </c>
+      <c r="G14" s="172"/>
+      <c r="H14" s="47">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52">
         <v>42736</v>
       </c>
@@ -3566,11 +3620,12 @@
         <v>84</v>
       </c>
       <c r="F15" s="172"/>
-      <c r="G15" s="47">
+      <c r="G15" s="172"/>
+      <c r="H15" s="47">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52">
         <v>42736</v>
       </c>
@@ -3585,7 +3640,8 @@
         <v>86</v>
       </c>
       <c r="F16" s="172"/>
-      <c r="G16" s="47">
+      <c r="G16" s="172"/>
+      <c r="H16" s="47">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RDM- 7800 - ShowConditions on Workbasket and Search Input fields (#566)
* RDM-7800 - ShowConditions on Workbasket and Search Input fields

* RDM-7800 - added validation for showConditions on Workbasket and Search Input fields

* RDM-7800 - unit tests for showConditions on Workbasket and Search Input fields parser

* RDM-7800 - updated test definition file to include showCondition on searchinput/workbasketinput tabs

* RDM-7800 - added more tests

* RDM-7800 - test fix - collection element order

* RDM-7800 - review comments

* RDM-7800 - review comments

* RDM-7800 - test fix

* RDM-7800 - updated Get api response

* RDM-7800 - functional tests json update

Co-authored-by: Ashley Noronha <ashleydeannoronha@gmail.com>
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sateesh/moj/workspace/ccd/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8482A7DC-2EA5-A947-8A69-2438D283D875}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BE840D-CF1B-3E43-AE22-E55F43201CCA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="16640" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="16640" tabRatio="500" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="366">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1165,6 +1165,15 @@
   </si>
   <si>
     <t>Last State Modified Date</t>
+  </si>
+  <si>
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;</t>
+  </si>
+  <si>
+    <t>Age="30"</t>
+  </si>
+  <si>
+    <t>ContectNumber="07777777777"</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1772,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="205">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2037,6 +2046,9 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -2706,10 +2718,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F1" sqref="F1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2718,12 +2730,12 @@
     <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="20.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="1" customWidth="1"/>
-    <col min="8" max="1026" width="8.83203125" customWidth="1"/>
+    <col min="5" max="7" width="20.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" customWidth="1"/>
+    <col min="9" max="1027" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>213</v>
       </c>
@@ -2738,9 +2750,10 @@
       </c>
       <c r="E1" s="47"/>
       <c r="F1" s="177"/>
-      <c r="G1" s="47"/>
-    </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="G1" s="177"/>
+      <c r="H1" s="47"/>
+    </row>
+    <row r="2" spans="1:8" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="48"/>
       <c r="B2" s="48"/>
       <c r="C2" s="49" t="s">
@@ -2752,14 +2765,17 @@
       <c r="E2" s="49" t="s">
         <v>215</v>
       </c>
-      <c r="F2" s="165" t="s">
+      <c r="F2" s="205" t="s">
+        <v>363</v>
+      </c>
+      <c r="G2" s="165" t="s">
         <v>332</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="H2" s="49" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="50" t="s">
         <v>7</v>
       </c>
@@ -2775,14 +2791,17 @@
       <c r="E3" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="124" t="s">
+      <c r="F3" s="161" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="124" t="s">
         <v>247</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="H3" s="50" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="52">
         <v>42736</v>
       </c>
@@ -2797,11 +2816,12 @@
         <v>46</v>
       </c>
       <c r="F4" s="172"/>
-      <c r="G4" s="47">
+      <c r="G4" s="172"/>
+      <c r="H4" s="47">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52">
         <v>42736</v>
       </c>
@@ -2816,11 +2836,12 @@
         <v>53</v>
       </c>
       <c r="F5" s="172"/>
-      <c r="G5" s="47">
+      <c r="G5" s="172"/>
+      <c r="H5" s="47">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="52">
         <v>42736</v>
       </c>
@@ -2835,11 +2856,12 @@
         <v>55</v>
       </c>
       <c r="F6" s="172"/>
-      <c r="G6" s="47">
+      <c r="G6" s="172"/>
+      <c r="H6" s="47">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
         <v>42736</v>
       </c>
@@ -2853,14 +2875,15 @@
       <c r="E7" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="172" t="s">
+      <c r="F7" s="172"/>
+      <c r="G7" s="172" t="s">
         <v>249</v>
       </c>
-      <c r="G7" s="47">
+      <c r="H7" s="47">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52">
         <v>42736</v>
       </c>
@@ -2875,11 +2898,12 @@
         <v>53</v>
       </c>
       <c r="F8" s="172"/>
-      <c r="G8" s="47">
+      <c r="G8" s="172"/>
+      <c r="H8" s="47">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52">
         <v>42736</v>
       </c>
@@ -2894,11 +2918,12 @@
         <v>55</v>
       </c>
       <c r="F9" s="172"/>
-      <c r="G9" s="47">
+      <c r="G9" s="172"/>
+      <c r="H9" s="47">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52">
         <v>42736</v>
       </c>
@@ -2913,11 +2938,12 @@
         <v>72</v>
       </c>
       <c r="F10" s="172"/>
-      <c r="G10" s="47">
+      <c r="G10" s="172"/>
+      <c r="H10" s="47">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52">
         <v>42736</v>
       </c>
@@ -2932,11 +2958,12 @@
         <v>75</v>
       </c>
       <c r="F11" s="172"/>
-      <c r="G11" s="47">
+      <c r="G11" s="172"/>
+      <c r="H11" s="47">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52">
         <v>42736</v>
       </c>
@@ -2951,11 +2978,12 @@
         <v>77</v>
       </c>
       <c r="F12" s="172"/>
-      <c r="G12" s="47">
+      <c r="G12" s="172"/>
+      <c r="H12" s="47">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52">
         <v>42736</v>
       </c>
@@ -2970,11 +2998,12 @@
         <v>79</v>
       </c>
       <c r="F13" s="172"/>
-      <c r="G13" s="47">
+      <c r="G13" s="172"/>
+      <c r="H13" s="47">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52">
         <v>42736</v>
       </c>
@@ -2989,11 +3018,12 @@
         <v>82</v>
       </c>
       <c r="F14" s="172"/>
-      <c r="G14" s="47">
+      <c r="G14" s="172"/>
+      <c r="H14" s="47">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52">
         <v>42736</v>
       </c>
@@ -3008,11 +3038,12 @@
         <v>84</v>
       </c>
       <c r="F15" s="172"/>
-      <c r="G15" s="47">
+      <c r="G15" s="172"/>
+      <c r="H15" s="47">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52">
         <v>42736</v>
       </c>
@@ -3026,8 +3057,11 @@
       <c r="E16" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="172"/>
-      <c r="G16" s="47">
+      <c r="F16" s="172" t="s">
+        <v>364</v>
+      </c>
+      <c r="G16" s="172"/>
+      <c r="H16" s="47">
         <v>10</v>
       </c>
     </row>
@@ -3044,7 +3078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -3264,10 +3298,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3276,12 +3310,12 @@
     <col min="2" max="2" width="15.33203125" style="55" customWidth="1"/>
     <col min="3" max="3" width="29.83203125" style="55" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" style="55" customWidth="1"/>
-    <col min="5" max="6" width="20.1640625" style="55" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="55" customWidth="1"/>
-    <col min="8" max="1026" width="8.83203125" customWidth="1"/>
+    <col min="5" max="7" width="20.1640625" style="55" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="55" customWidth="1"/>
+    <col min="9" max="1027" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>219</v>
       </c>
@@ -3295,10 +3329,11 @@
         <v>3</v>
       </c>
       <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="F1" s="177"/>
       <c r="G1" s="60"/>
-    </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="H1" s="60"/>
+    </row>
+    <row r="2" spans="1:8" ht="80" x14ac:dyDescent="0.15">
       <c r="A2" s="61"/>
       <c r="B2" s="61"/>
       <c r="C2" s="62" t="s">
@@ -3310,14 +3345,17 @@
       <c r="E2" s="62" t="s">
         <v>222</v>
       </c>
-      <c r="F2" s="165" t="s">
+      <c r="F2" s="205" t="s">
+        <v>363</v>
+      </c>
+      <c r="G2" s="165" t="s">
         <v>332</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="H2" s="62" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="63" t="s">
         <v>7</v>
       </c>
@@ -3333,14 +3371,17 @@
       <c r="E3" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="124" t="s">
+      <c r="F3" s="161" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="124" t="s">
         <v>247</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="H3" s="63" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="52">
         <v>42736</v>
       </c>
@@ -3355,11 +3396,12 @@
         <v>46</v>
       </c>
       <c r="F4" s="172"/>
-      <c r="G4" s="47">
+      <c r="G4" s="172"/>
+      <c r="H4" s="47">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52">
         <v>42736</v>
       </c>
@@ -3373,12 +3415,13 @@
       <c r="E5" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="172"/>
-      <c r="G5" s="47">
+      <c r="F5" s="53"/>
+      <c r="G5" s="172"/>
+      <c r="H5" s="47">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="52">
         <v>42736</v>
       </c>
@@ -3393,11 +3436,12 @@
         <v>55</v>
       </c>
       <c r="F6" s="172"/>
-      <c r="G6" s="47">
+      <c r="G6" s="172"/>
+      <c r="H6" s="47">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
         <v>42736</v>
       </c>
@@ -3411,14 +3455,15 @@
       <c r="E7" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="172" t="s">
+      <c r="F7" s="172"/>
+      <c r="G7" s="172" t="s">
         <v>249</v>
       </c>
-      <c r="G7" s="47">
+      <c r="H7" s="47">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52">
         <v>42736</v>
       </c>
@@ -3433,11 +3478,12 @@
         <v>53</v>
       </c>
       <c r="F8" s="172"/>
-      <c r="G8" s="47">
+      <c r="G8" s="172"/>
+      <c r="H8" s="47">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52">
         <v>42736</v>
       </c>
@@ -3452,11 +3498,12 @@
         <v>55</v>
       </c>
       <c r="F9" s="172"/>
-      <c r="G9" s="47">
+      <c r="G9" s="172"/>
+      <c r="H9" s="47">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52">
         <v>42736</v>
       </c>
@@ -3471,11 +3518,12 @@
         <v>72</v>
       </c>
       <c r="F10" s="172"/>
-      <c r="G10" s="47">
+      <c r="G10" s="172"/>
+      <c r="H10" s="47">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52">
         <v>42736</v>
       </c>
@@ -3490,11 +3538,12 @@
         <v>75</v>
       </c>
       <c r="F11" s="172"/>
-      <c r="G11" s="47">
+      <c r="G11" s="172"/>
+      <c r="H11" s="47">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52">
         <v>42736</v>
       </c>
@@ -3509,11 +3558,12 @@
         <v>77</v>
       </c>
       <c r="F12" s="172"/>
-      <c r="G12" s="47">
+      <c r="G12" s="172"/>
+      <c r="H12" s="47">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52">
         <v>42736</v>
       </c>
@@ -3528,11 +3578,12 @@
         <v>79</v>
       </c>
       <c r="F13" s="172"/>
-      <c r="G13" s="47">
+      <c r="G13" s="172"/>
+      <c r="H13" s="47">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52">
         <v>42736</v>
       </c>
@@ -3546,12 +3597,15 @@
       <c r="E14" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="172"/>
-      <c r="G14" s="47">
+      <c r="F14" s="53" t="s">
+        <v>365</v>
+      </c>
+      <c r="G14" s="172"/>
+      <c r="H14" s="47">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52">
         <v>42736</v>
       </c>
@@ -3566,11 +3620,12 @@
         <v>84</v>
       </c>
       <c r="F15" s="172"/>
-      <c r="G15" s="47">
+      <c r="G15" s="172"/>
+      <c r="H15" s="47">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52">
         <v>42736</v>
       </c>
@@ -3585,7 +3640,8 @@
         <v>86</v>
       </c>
       <c r="F16" s="172"/>
-      <c r="G16" s="47">
+      <c r="G16" s="172"/>
+      <c r="H16" s="47">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RDM-7575 merged develop into branch and resolved issues
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sateesh/moj/workspace/ccd/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BE840D-CF1B-3E43-AE22-E55F43201CCA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A217D177-29A7-1045-9BD7-F8B67F070DA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28060" windowHeight="16640" tabRatio="500" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35200" windowHeight="19700" tabRatio="500" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="365">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1027,9 +1027,6 @@
   </si>
   <si>
     <t>MaxLength: 1000</t>
-  </si>
-  <si>
-    <t>#TABLE(Title, FirstName, MiddleName)</t>
   </si>
   <si>
     <t>ReferenceCollectionTab</t>
@@ -2753,7 +2750,7 @@
       <c r="G1" s="177"/>
       <c r="H1" s="47"/>
     </row>
-    <row r="2" spans="1:8" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="80" x14ac:dyDescent="0.15">
       <c r="A2" s="48"/>
       <c r="B2" s="48"/>
       <c r="C2" s="49" t="s">
@@ -2766,10 +2763,10 @@
         <v>215</v>
       </c>
       <c r="F2" s="205" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G2" s="165" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H2" s="49" t="s">
         <v>156</v>
@@ -3058,7 +3055,7 @@
         <v>86</v>
       </c>
       <c r="F16" s="172" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G16" s="172"/>
       <c r="H16" s="47">
@@ -3123,7 +3120,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="165" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>156</v>
@@ -3218,10 +3215,10 @@
         <v>24</v>
       </c>
       <c r="D7" s="178" t="s">
+        <v>360</v>
+      </c>
+      <c r="E7" s="204" t="s">
         <v>361</v>
-      </c>
-      <c r="E7" s="204" t="s">
-        <v>362</v>
       </c>
       <c r="F7" s="204"/>
       <c r="G7" s="203">
@@ -3300,7 +3297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
@@ -3346,10 +3343,10 @@
         <v>222</v>
       </c>
       <c r="F2" s="205" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G2" s="165" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H2" s="62" t="s">
         <v>156</v>
@@ -3598,7 +3595,7 @@
         <v>82</v>
       </c>
       <c r="F14" s="53" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G14" s="172"/>
       <c r="H14" s="47">
@@ -3703,7 +3700,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="165" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G2" s="64" t="s">
         <v>156</v>
@@ -3861,8 +3858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3928,7 +3925,7 @@
         <v>4</v>
       </c>
       <c r="I2" s="165" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J2" s="164" t="s">
         <v>226</v>
@@ -4125,16 +4122,16 @@
         <v>232</v>
       </c>
       <c r="E8" s="119" t="s">
+        <v>329</v>
+      </c>
+      <c r="F8" s="172" t="s">
         <v>330</v>
-      </c>
-      <c r="F8" s="172" t="s">
-        <v>331</v>
       </c>
       <c r="G8" s="99">
         <v>4</v>
       </c>
       <c r="H8" s="119" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I8" s="119"/>
       <c r="J8" s="99">
@@ -4156,7 +4153,7 @@
         <v>232</v>
       </c>
       <c r="E9" s="150" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F9" s="172" t="s">
         <v>317</v>
@@ -4173,9 +4170,7 @@
       </c>
       <c r="K9" s="99"/>
       <c r="L9" s="99"/>
-      <c r="M9" s="173" t="s">
-        <v>319</v>
-      </c>
+      <c r="M9" s="173"/>
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="171">
@@ -8219,7 +8214,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="119" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E12" s="139" t="s">
         <v>253</v>
@@ -8609,7 +8604,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="185" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B1" s="186" t="s">
         <v>1</v>
@@ -8628,19 +8623,19 @@
       <c r="A2" s="190"/>
       <c r="B2" s="190"/>
       <c r="C2" s="191" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="191" t="s">
         <v>339</v>
       </c>
-      <c r="D2" s="191" t="s">
+      <c r="E2" s="191" t="s">
         <v>340</v>
       </c>
-      <c r="E2" s="191" t="s">
+      <c r="F2" s="191" t="s">
         <v>341</v>
       </c>
-      <c r="F2" s="191" t="s">
+      <c r="G2" s="191" t="s">
         <v>342</v>
-      </c>
-      <c r="G2" s="191" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -8795,7 +8790,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8822,10 +8817,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -8840,16 +8835,16 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>353</v>
-      </c>
       <c r="E3" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="7"/>
@@ -8864,16 +8859,16 @@
         <v>12</v>
       </c>
       <c r="B4" s="117" t="s">
+        <v>356</v>
+      </c>
+      <c r="C4" s="201" t="s">
+        <v>359</v>
+      </c>
+      <c r="D4" s="201" t="s">
         <v>357</v>
       </c>
-      <c r="C4" s="201" t="s">
-        <v>360</v>
-      </c>
-      <c r="D4" s="201" t="s">
+      <c r="E4" s="200" t="s">
         <v>358</v>
-      </c>
-      <c r="E4" s="200" t="s">
-        <v>359</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="3"/>
@@ -14026,7 +14021,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="156" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B1" s="157" t="s">
         <v>1</v>
@@ -14041,10 +14036,10 @@
     <row r="2" spans="1:4" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="160"/>
       <c r="B2" s="160" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="160" t="s">
         <v>322</v>
-      </c>
-      <c r="C2" s="160" t="s">
-        <v>323</v>
       </c>
       <c r="D2" s="160"/>
     </row>
@@ -14053,7 +14048,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="161" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C3" s="161" t="s">
         <v>193</v>
@@ -14065,7 +14060,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="125" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C4" s="125" t="s">
         <v>52</v>
@@ -14077,7 +14072,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="125" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C5" s="125" t="s">
         <v>52</v>
@@ -14089,10 +14084,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="163" t="s">
+        <v>325</v>
+      </c>
+      <c r="C6" s="125" t="s">
         <v>326</v>
-      </c>
-      <c r="C6" s="125" t="s">
-        <v>327</v>
       </c>
       <c r="D6" s="163"/>
     </row>
@@ -15105,14 +15100,14 @@
         <v>24</v>
       </c>
       <c r="D16" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>328</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>329</v>
       </c>
       <c r="F16" s="99"/>
       <c r="G16" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H16" s="99"/>
       <c r="I16" s="99"/>
@@ -15181,14 +15176,14 @@
         <v>24</v>
       </c>
       <c r="D18" s="179" t="s">
+        <v>332</v>
+      </c>
+      <c r="E18" s="179" t="s">
         <v>333</v>
-      </c>
-      <c r="E18" s="179" t="s">
-        <v>334</v>
       </c>
       <c r="F18" s="180"/>
       <c r="G18" s="178" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H18" s="179"/>
       <c r="I18" s="180"/>
@@ -15218,14 +15213,14 @@
         <v>24</v>
       </c>
       <c r="D19" s="179" t="s">
+        <v>335</v>
+      </c>
+      <c r="E19" s="179" t="s">
         <v>336</v>
-      </c>
-      <c r="E19" s="179" t="s">
-        <v>337</v>
       </c>
       <c r="F19" s="180"/>
       <c r="G19" s="178" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H19" s="178" t="s">
         <v>88</v>
@@ -16432,7 +16427,7 @@
         <v>116</v>
       </c>
       <c r="H2" s="198" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>35</v>
@@ -16528,7 +16523,7 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="150" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -16564,7 +16559,7 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="150" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -16600,7 +16595,7 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="150" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -16636,7 +16631,7 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="150" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -16674,7 +16669,7 @@
         <v>127</v>
       </c>
       <c r="H8" s="150" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -18410,8 +18405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView showGridLines="0" topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18899,7 +18894,7 @@
       </c>
       <c r="H12" s="113"/>
       <c r="I12" s="33" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J12" s="113">
         <v>1</v>
@@ -19037,9 +19032,7 @@
       <c r="K15" s="99" t="s">
         <v>267</v>
       </c>
-      <c r="L15" s="155" t="s">
-        <v>319</v>
-      </c>
+      <c r="L15" s="155"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>

</xml_diff>

<commit_message>
RDM-9024 fixed failing test
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A217D177-29A7-1045-9BD7-F8B67F070DA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94A6D44-AEF9-AF4D-848C-12A476A9BE9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35200" windowHeight="19700" tabRatio="500" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35200" windowHeight="19700" tabRatio="500" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -3655,9 +3655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3858,7 +3856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -18405,7 +18403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RDM-12828 - add TTL increment column in case event
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-6719.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08217A6-9842-A943-A600-278455E9A3F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA1D792-B122-9C41-AD6F-7A8065F050CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="42740" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20560" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="365">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1168,6 +1168,9 @@
   <si>
     <t>Must match ID of AccessProfile or CaseRole.  If it doesn’t have a Row below that means no access to.
 MaxLength: 100.</t>
+  </si>
+  <si>
+    <t>TTLIncrement</t>
   </si>
 </sst>
 </file>
@@ -2091,6 +2094,169 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -2099,6 +2265,283 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -2112,9 +2555,403 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
         <color auto="1"/>
-        <name val="Calibri"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
@@ -2348,13 +3185,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -2388,6 +3218,13 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2398,11 +3235,10 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FFFFC000"/>
-        <name val="Arial"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2424,612 +3260,6 @@
         <bottom/>
       </border>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -3107,243 +3337,16 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FFFFC000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="ccd-definition-tab" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ccd-definition-tab" pivot="0" count="7" xr9:uid="{4671BC98-5267-1349-9483-85BCB1E0571F}">
-      <tableStyleElement type="wholeTable" dxfId="48"/>
-      <tableStyleElement type="headerRow" dxfId="47"/>
-      <tableStyleElement type="totalRow" dxfId="46"/>
-      <tableStyleElement type="firstColumn" dxfId="45"/>
-      <tableStyleElement type="lastColumn" dxfId="44"/>
-      <tableStyleElement type="firstRowStripe" dxfId="43"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="42"/>
+      <tableStyleElement type="wholeTable" dxfId="58"/>
+      <tableStyleElement type="headerRow" dxfId="57"/>
+      <tableStyleElement type="totalRow" dxfId="56"/>
+      <tableStyleElement type="firstColumn" dxfId="55"/>
+      <tableStyleElement type="lastColumn" dxfId="54"/>
+      <tableStyleElement type="firstRowStripe" dxfId="53"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="52"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3478,24 +3481,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F253DF98-DCCE-C64A-8E95-4EF1549FE3C1}" name="SearchInputFields" displayName="SearchInputFields" ref="A3:H21" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="10" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F253DF98-DCCE-C64A-8E95-4EF1549FE3C1}" name="SearchInputFields" displayName="SearchInputFields" ref="A3:H21" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48">
   <autoFilter ref="A3:H21" xr:uid="{20F59D09-4EE5-3046-8BE0-0ED46E61247A}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{4BF963A9-4D42-6D4C-AD25-1F071447896C}" name="LiveFrom" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{4A035A8A-DFD5-6D43-9D62-61C2BAABAF8B}" name="LiveTo" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{1DD7918C-E1B8-544F-9EFE-2D3FCCB1503B}" name="CaseTypeID" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{3ABDE47D-0573-9B42-B77E-387F16CEA06E}" name="CaseFieldID" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{D9C695D5-3D29-8F4F-AB53-BAC95B9010B8}" name="Label" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{7F82DEE9-3A70-724A-81D7-513F9CD476F6}" name="FieldShowCondition" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{4CD70F21-CE0B-7848-B441-B068D3762E3B}" name="AccessProfile" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{CC4C0933-CE5A-984B-8977-6F39CE38BA00}" name="DisplayOrder" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{4BF963A9-4D42-6D4C-AD25-1F071447896C}" name="LiveFrom" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{4A035A8A-DFD5-6D43-9D62-61C2BAABAF8B}" name="LiveTo" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{1DD7918C-E1B8-544F-9EFE-2D3FCCB1503B}" name="CaseTypeID" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{3ABDE47D-0573-9B42-B77E-387F16CEA06E}" name="CaseFieldID" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{D9C695D5-3D29-8F4F-AB53-BAC95B9010B8}" name="Label" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{7F82DEE9-3A70-724A-81D7-513F9CD476F6}" name="FieldShowCondition" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{4CD70F21-CE0B-7848-B441-B068D3762E3B}" name="AccessProfile" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{CC4C0933-CE5A-984B-8977-6F39CE38BA00}" name="DisplayOrder" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="ccd-definition-tab" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BDF3738-D63B-974D-862C-A17514FF2272}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E15" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" headerRowBorderDxfId="54" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BDF3738-D63B-974D-862C-A17514FF2272}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E15" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
   <autoFilter ref="A3:E15" xr:uid="{9DA09A83-7E1F-6C4F-924F-69B9B42E2D57}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3504,18 +3507,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CF561400-70B6-024F-9231-2AC08879D8A2}" name="LiveFrom" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{EE426005-5BA6-5944-80AD-29D83230DA05}" name="LiveTo" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{8AC6FCF7-AC7F-9F40-96F8-C4E1728D2226}" name="CaseTypeID" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{44A822AB-375A-6E40-BA89-128A9D13D67F}" name="AccessProfile" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{3D716DCF-D533-FC42-916B-97855487DF24}" name="CRUD" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{CF561400-70B6-024F-9231-2AC08879D8A2}" name="LiveFrom" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{EE426005-5BA6-5944-80AD-29D83230DA05}" name="LiveTo" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{8AC6FCF7-AC7F-9F40-96F8-C4E1728D2226}" name="CaseTypeID" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{44A822AB-375A-6E40-BA89-128A9D13D67F}" name="AccessProfile" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{3D716DCF-D533-FC42-916B-97855487DF24}" name="CRUD" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="ccd-definition-tab" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{410CF670-ABF7-8F4C-B79E-8CDA1B49A010}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F38" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" headerRowBorderDxfId="40" tableBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{410CF670-ABF7-8F4C-B79E-8CDA1B49A010}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F38" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27">
   <autoFilter ref="A3:F38" xr:uid="{63A93BBC-6E57-4044-8076-EE674C814033}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3525,19 +3528,19 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7210A091-D35B-644F-80F4-5D9286B43C71}" name="LiveFrom" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{394C4375-AC7E-3145-A439-EB53364B1104}" name="LiveTo" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{69292D9C-5B41-7A4C-B3AB-DAE170F9766E}" name="CaseTypeID" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{E69AE292-3C6C-A848-AD2F-D9EDF81CBAEC}" name="CaseFieldID" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{F1080042-6B05-234D-893D-3CBDD782FD94}" name="AccessProfile" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{98F4D225-4710-ED49-9022-5E80226865DA}" name="CRUD" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{7210A091-D35B-644F-80F4-5D9286B43C71}" name="LiveFrom" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{394C4375-AC7E-3145-A439-EB53364B1104}" name="LiveTo" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{69292D9C-5B41-7A4C-B3AB-DAE170F9766E}" name="CaseTypeID" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{E69AE292-3C6C-A848-AD2F-D9EDF81CBAEC}" name="CaseFieldID" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{F1080042-6B05-234D-893D-3CBDD782FD94}" name="AccessProfile" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{98F4D225-4710-ED49-9022-5E80226865DA}" name="CRUD" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="ccd-definition-tab" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6657A5F7-9B08-8549-8FAA-4A42233CC96B}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G17" totalsRowShown="0" headerRowDxfId="58" headerRowCellStyle="Normal 2 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6657A5F7-9B08-8549-8FAA-4A42233CC96B}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G17" totalsRowShown="0" headerRowDxfId="20" headerRowCellStyle="Normal 2 3">
   <autoFilter ref="A3:G17" xr:uid="{870B772B-2204-9347-B622-FE2BF808A91A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3561,7 +3564,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{96A76EEC-A661-3C42-864F-202B3AF6D81A}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F24" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="30" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{96A76EEC-A661-3C42-864F-202B3AF6D81A}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
   <autoFilter ref="A3:F24" xr:uid="{7A611F98-E4F4-FC41-BC78-79167A32CDD7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3571,27 +3574,27 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{60C5E7EF-E4AE-354A-B18F-114FB4222A48}" name="LiveFrom" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{9B5093F6-BC5E-7343-BFAC-46214387E398}" name="LiveTo" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{56696EE5-DD05-0849-934B-6A412A688AA7}" name="CaseTypeID" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{9E9534C2-3382-EF41-846B-735ACE8701CA}" name="CaseEventID" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{7C21B2E1-CDE6-C941-9C05-CF970412474A}" name="AccessProfile" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{3AB322BC-4312-0A43-8353-0FCC813987C8}" name="CRUD" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{60C5E7EF-E4AE-354A-B18F-114FB4222A48}" name="LiveFrom" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{9B5093F6-BC5E-7343-BFAC-46214387E398}" name="LiveTo" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{56696EE5-DD05-0849-934B-6A412A688AA7}" name="CaseTypeID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{9E9534C2-3382-EF41-846B-735ACE8701CA}" name="CaseEventID" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{7C21B2E1-CDE6-C941-9C05-CF970412474A}" name="AccessProfile" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{3AB322BC-4312-0A43-8353-0FCC813987C8}" name="CRUD" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="ccd-definition-tab" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BAB46232-7BE5-A84F-BD88-2B7298B12F7B}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F22" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="20" tableBorderDxfId="21" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BAB46232-7BE5-A84F-BD88-2B7298B12F7B}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F22" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
   <autoFilter ref="A3:F22" xr:uid="{A197022F-C363-1F48-84FD-3ADAF66C7619}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5173758A-AAEB-F543-9FE6-B1CC079D4E9C}" name="LiveFrom" dataDxfId="19" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="2" xr3:uid="{97169C69-B0B2-C64B-BD76-2CDED6BE1FD0}" name="LiveTo" dataDxfId="18" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="3" xr3:uid="{374ABD1A-6DD9-2742-BBD9-75789C7CCA8E}" name="CaseTypeID" dataDxfId="17" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="4" xr3:uid="{2B2DC372-E563-1146-9008-6A00F93FEB5A}" name="CaseStateID" dataDxfId="16" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="5" xr3:uid="{8EC6D8AD-050A-8747-9AC2-5ECCB9E07082}" name="AccessProfile" dataDxfId="15" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="6" xr3:uid="{D299DF40-9A0E-5C47-91BE-1DF3BB4C5BA1}" name="CRUD" dataDxfId="14" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="1" xr3:uid="{5173758A-AAEB-F543-9FE6-B1CC079D4E9C}" name="LiveFrom" dataDxfId="5" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="2" xr3:uid="{97169C69-B0B2-C64B-BD76-2CDED6BE1FD0}" name="LiveTo" dataDxfId="4" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="3" xr3:uid="{374ABD1A-6DD9-2742-BBD9-75789C7CCA8E}" name="CaseTypeID" dataDxfId="3" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="4" xr3:uid="{2B2DC372-E563-1146-9008-6A00F93FEB5A}" name="CaseStateID" dataDxfId="2" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="5" xr3:uid="{8EC6D8AD-050A-8747-9AC2-5ECCB9E07082}" name="AccessProfile" dataDxfId="1" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="6" xr3:uid="{D299DF40-9A0E-5C47-91BE-1DF3BB4C5BA1}" name="CRUD" dataDxfId="0" dataCellStyle="Explanatory Text"/>
   </tableColumns>
   <tableStyleInfo name="ccd-definition-tab" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4124,7 +4127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -18994,8 +18997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -19175,7 +19178,9 @@
       <c r="T3" s="101" t="s">
         <v>291</v>
       </c>
-      <c r="U3" s="8"/>
+      <c r="U3" s="8" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="4" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
@@ -19226,7 +19231,9 @@
       <c r="T4" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="U4" s="4"/>
+      <c r="U4" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
@@ -19273,7 +19280,9 @@
         <v>278</v>
       </c>
       <c r="T5" s="93"/>
-      <c r="U5" s="4"/>
+      <c r="U5" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
@@ -19316,7 +19325,9 @@
       <c r="R6" s="99"/>
       <c r="S6" s="4"/>
       <c r="T6" s="93"/>
-      <c r="U6" s="4"/>
+      <c r="U6" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">

</xml_diff>